<commit_message>
NewBranch Commit - Updates to PageObjects
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/pageobjects/PageObjects.xlsx
+++ b/src/test/resources/testdata/pageobjects/PageObjects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UB217ZA\Downloads\Github Clone NGTP\ExcelVersionNew\src\test\resources\testdata\pageobjects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UB217ZA\Downloads\Github Clone NGTP\VersionControlExcel\src\test\resources\testdata\pageobjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA75AA4-D18C-48C8-BD69-7313B4A27399}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB21D245-F7FB-46FE-91EC-011F9C3C649A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,9 +96,6 @@
     <t>select</t>
   </si>
   <si>
-    <t>search_dropdown</t>
-  </si>
-  <si>
     <t>option</t>
   </si>
   <si>
@@ -283,6 +280,9 @@
   </si>
   <si>
     <t>searchDropdownBox</t>
+  </si>
+  <si>
+    <t>search_dropdown1</t>
   </si>
 </sst>
 </file>
@@ -669,7 +669,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -772,68 +772,68 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" t="s">
+      <c r="F9" t="s">
         <v>26</v>
-      </c>
-      <c r="F9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
         <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
         <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
         <v>32</v>
-      </c>
-      <c r="E12" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
         <v>34</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
         <v>36</v>
-      </c>
-      <c r="E14" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F7 A9:F14 A8:C8 E8:F8" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:F7 A9:F14 A8 E8:F8 C8" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -862,10 +862,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
         <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>39</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -874,13 +874,13 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
         <v>40</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>41</v>
-      </c>
-      <c r="K1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -888,10 +888,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
         <v>43</v>
-      </c>
-      <c r="G2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -899,10 +899,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" t="s">
         <v>45</v>
-      </c>
-      <c r="G3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -910,10 +910,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" t="s">
         <v>47</v>
-      </c>
-      <c r="G4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -921,10 +921,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
         <v>49</v>
-      </c>
-      <c r="G5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -932,10 +932,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
         <v>51</v>
-      </c>
-      <c r="G6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -943,10 +943,10 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" t="s">
         <v>53</v>
-      </c>
-      <c r="G7" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -954,10 +954,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s">
         <v>55</v>
-      </c>
-      <c r="G8" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1000,7 +1000,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1012,143 +1012,143 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G12" s="2"/>
     </row>
@@ -1157,26 +1157,26 @@
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1184,15 +1184,15 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="2"/>

</xml_diff>

<commit_message>
Main Branch - Updates to Pageobjects
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/pageobjects/PageObjects.xlsx
+++ b/src/test/resources/testdata/pageobjects/PageObjects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UB217ZA\Downloads\Github Clone NGTP\ExcelVersionNew\src\test\resources\testdata\pageobjects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UB217ZA\Downloads\Github Clone NGTP\ExcelVersion\src\test\resources\testdata\pageobjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA75AA4-D18C-48C8-BD69-7313B4A27399}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857BFCEE-9928-4F07-94ED-927D4DD1208D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,9 +96,6 @@
     <t>select</t>
   </si>
   <si>
-    <t>search_dropdown</t>
-  </si>
-  <si>
     <t>option</t>
   </si>
   <si>
@@ -283,6 +280,9 @@
   </si>
   <si>
     <t>searchDropdownBox</t>
+  </si>
+  <si>
+    <t>search_dropdown1</t>
   </si>
 </sst>
 </file>
@@ -669,7 +669,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -772,68 +772,68 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" t="s">
+      <c r="F9" t="s">
         <v>26</v>
-      </c>
-      <c r="F9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
         <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
         <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
         <v>32</v>
-      </c>
-      <c r="E12" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
         <v>34</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
         <v>36</v>
-      </c>
-      <c r="E14" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F7 A9:F14 A8:C8 E8:F8" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:F7 A9:F14 A8 E8:F8 C8" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -862,10 +862,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
         <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>39</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -874,13 +874,13 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
         <v>40</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>41</v>
-      </c>
-      <c r="K1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -888,10 +888,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
         <v>43</v>
-      </c>
-      <c r="G2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -899,10 +899,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" t="s">
         <v>45</v>
-      </c>
-      <c r="G3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -910,10 +910,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" t="s">
         <v>47</v>
-      </c>
-      <c r="G4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -921,10 +921,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
         <v>49</v>
-      </c>
-      <c r="G5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -932,10 +932,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
         <v>51</v>
-      </c>
-      <c r="G6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -943,10 +943,10 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" t="s">
         <v>53</v>
-      </c>
-      <c r="G7" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -954,10 +954,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s">
         <v>55</v>
-      </c>
-      <c r="G8" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1000,7 +1000,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1012,143 +1012,143 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G12" s="2"/>
     </row>
@@ -1157,26 +1157,26 @@
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1184,15 +1184,15 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="2"/>

</xml_diff>

<commit_message>
NewBranch Pageobjects csv and xml commit
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/pageobjects/PageObjects.xlsx
+++ b/src/test/resources/testdata/pageobjects/PageObjects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UB217ZA\Downloads\Github Clone NGTP\VersionControlExcel\src\test\resources\testdata\pageobjects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UB217ZA\Downloads\Github Clone NGTP\ExcelVersion\src\test\resources\testdata\pageobjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB21D245-F7FB-46FE-91EC-011F9C3C649A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857BFCEE-9928-4F07-94ED-927D4DD1208D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
Main Branch - Updates to Pageobjects xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/pageobjects/PageObjects.xlsx
+++ b/src/test/resources/testdata/pageobjects/PageObjects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UB217ZA\Downloads\Github Clone NGTP\ExcelVersion\src\test\resources\testdata\pageobjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857BFCEE-9928-4F07-94ED-927D4DD1208D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B62354-C68D-43CE-8E52-6B0C815DB294}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -282,7 +282,7 @@
     <t>searchDropdownBox</t>
   </si>
   <si>
-    <t>search_dropdown1</t>
+    <t>search_dropdown</t>
   </si>
 </sst>
 </file>

</xml_diff>